<commit_message>
recoding pass 2 done, with super domains
</commit_message>
<xml_diff>
--- a/data/domains/domain_recodes.xlsx
+++ b/data/domains/domain_recodes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkolendo/Documents/r_projects/scientist_surveys/data/domains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7F52966-7A6D-4249-907A-A2A059C41C72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF770606-934C-0E49-B69E-3ED1A28917E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32640" yWindow="-980" windowWidth="28040" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="domain_mapping" sheetId="4" r:id="rId1"/>
-    <sheet name="recoded_domain_mapping" sheetId="5" r:id="rId2"/>
+    <sheet name="domain_recodes" sheetId="5" r:id="rId2"/>
     <sheet name="survey_one_domains" sheetId="3" r:id="rId3"/>
     <sheet name="survey_two_domains" sheetId="1" r:id="rId4"/>
     <sheet name="survey_three_domains" sheetId="2" r:id="rId5"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="303">
   <si>
     <t>Agriculture and Natural Resources</t>
   </si>
@@ -956,6 +956,18 @@
   </si>
   <si>
     <t>Health Sciences</t>
+  </si>
+  <si>
+    <t>super_domain_name</t>
+  </si>
+  <si>
+    <t>Physical science</t>
+  </si>
+  <si>
+    <t>Natural science</t>
+  </si>
+  <si>
+    <t>Social science</t>
   </si>
 </sst>
 </file>
@@ -4037,10 +4049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194C5BFB-44F4-CD4A-A319-2EAD73DF9606}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4049,95 +4061,128 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>296</v>
       </c>
       <c r="B1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>293</v>
       </c>
       <c r="B11">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -4145,116 +4190,158 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B15">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B19">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B20">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B21">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>294</v>
       </c>
       <c r="B23">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>295</v>
       </c>
       <c r="B24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>292</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>298</v>
       </c>
       <c r="B26">
         <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>